<commit_message>
V1: Migration POST ALL E2RH : +cotisation:just_log +idccToOpcc +emploiCCN +formJuridique +Makefile +placeholder:signataire +cumuls:add_and_modification +silaeGet +moreLogs
</commit_message>
<xml_diff>
--- a/data/in/idcc_opcc.xlsx
+++ b/data/in/idcc_opcc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://e2rh-my.sharepoint.com/personal/v_coru_e2rh_fr/Documents/workspace/open-paye-migration/data/in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_5FF111AAD310DA7C037A3911595ED87656CCA57C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08E8DBB1-A57E-4A46-AF0D-EE759AA31A2F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_5FF111AAD310DA7C037A3911595ED87656CCA57C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2737529-DC0E-4DC7-B1E9-7017C4E652F0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B383"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="N264" sqref="N264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,7 +4726,7 @@
         <v>439</v>
       </c>
       <c r="B375" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
@@ -4734,7 +4734,7 @@
         <v>439</v>
       </c>
       <c r="B376" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
         <v>439</v>
       </c>
       <c r="B377" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
         <v>439</v>
       </c>
       <c r="B378" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>